<commit_message>
Lesson05 - Part IV - Finished Excel Data Table Example
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Excel.xlsx
+++ b/src/test/resources/testdata/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limanaj/eclipse-workspace/TestNGFramework8/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabah\eclipse-workspace-8\CucumberFramework8\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1142D5-3A1B-C846-B962-F369812E9B0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8577C5A7-3739-46EE-9314-9E2CDBF67CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="1460" windowWidth="22100" windowHeight="12200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33750" yWindow="720" windowWidth="20985" windowHeight="14760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Secret@123!!</t>
-  </si>
-  <si>
     <t>Mary</t>
   </si>
   <si>
@@ -65,17 +62,20 @@
     <t>Canadian Development Center</t>
   </si>
   <si>
-    <t>MaryAnn384</t>
-  </si>
-  <si>
-    <t>JohnSmith234</t>
+    <t>Secret@123!!ABC</t>
+  </si>
+  <si>
+    <t>JohnSmith2345005</t>
+  </si>
+  <si>
+    <t>MaryAnn3845500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -87,6 +87,14 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -108,14 +116,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,19 +462,19 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.875" customWidth="1"/>
+    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -480,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -488,30 +499,30 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +545,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -547,7 +558,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>